<commit_message>
Creating ui for SAP scripting
</commit_message>
<xml_diff>
--- a/templates/InstrumentSign_New.xlsx
+++ b/templates/InstrumentSign_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlam\OneDrive - Illumina, Inc\Documents\Github\Integration-1-Prep-Project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45AAEBA-8486-42D3-8330-D64A39C37BF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B85E7-25BA-41CD-A204-9875C70D5A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -66,10 +66,10 @@
     <t>CA 1.0</t>
   </si>
   <si>
-    <t>A01549</t>
-  </si>
-  <si>
-    <t>APXCAS2126010</t>
+    <t>A01593</t>
+  </si>
+  <si>
+    <t>APXCAS2131001</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>20565151</v>
+        <v>20578713</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="B7" s="21">
         <f>IF(MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3)=0,3,MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -903,45 +903,45 @@
     <row r="1" spans="2:4" ht="38.5" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="str">
         <f xml:space="preserve"> "PRO:"&amp;Input!B3</f>
-        <v>PRO:20565151</v>
+        <v>PRO:20578713</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="str">
         <f>B1</f>
-        <v>PRO:20565151</v>
+        <v>PRO:20578713</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="90.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="str">
         <f>Input!B4</f>
-        <v>A01549</v>
+        <v>A01593</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>A01549</v>
+        <v>A01593</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="str">
         <f>Input!B5</f>
-        <v>APXCAS2126010</v>
+        <v>APXCAS2131001</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="str">
         <f>B3</f>
-        <v>APXCAS2126010</v>
+        <v>APXCAS2131001</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="64.5" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="str">
         <f>B3</f>
-        <v>APXCAS2126010</v>
+        <v>APXCAS2131001</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="str">
         <f>D3</f>
-        <v>APXCAS2126010</v>
+        <v>APXCAS2131001</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
@@ -958,12 +958,12 @@
     <row r="6" spans="2:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="str">
         <f>"Cell# "&amp;Input!B7</f>
-        <v>Cell# 1</v>
+        <v>Cell# 3</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="10" t="str">
         <f>B6</f>
-        <v>Cell# 1</v>
+        <v>Cell# 3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SAP script feature
Added ui and auto script editting for SAP script.

Fixed problem where sometimes rows in material lists were split so serial numbers were being set to NaN.
</commit_message>
<xml_diff>
--- a/templates/InstrumentSign_New.xlsx
+++ b/templates/InstrumentSign_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlam\OneDrive - Illumina, Inc\Documents\Github\Integration-1-Prep-Project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237B85E7-25BA-41CD-A204-9875C70D5A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B85E75-BF82-4D00-A7FC-6A2296F921D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t>CA 1.0</t>
   </si>
   <si>
-    <t>A01593</t>
-  </si>
-  <si>
-    <t>APXCAS2131001</t>
+    <t>A01603</t>
+  </si>
+  <si>
+    <t>APXCAS2131011</t>
   </si>
 </sst>
 </file>
@@ -752,7 +752,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>20578713</v>
+        <v>20578803</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="B7" s="21">
         <f>IF(MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3)=0,3,MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -903,45 +903,45 @@
     <row r="1" spans="2:4" ht="38.5" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="str">
         <f xml:space="preserve"> "PRO:"&amp;Input!B3</f>
-        <v>PRO:20578713</v>
+        <v>PRO:20578803</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="str">
         <f>B1</f>
-        <v>PRO:20578713</v>
+        <v>PRO:20578803</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="90.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="str">
         <f>Input!B4</f>
-        <v>A01593</v>
+        <v>A01603</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>A01593</v>
+        <v>A01603</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="str">
         <f>Input!B5</f>
-        <v>APXCAS2131001</v>
+        <v>APXCAS2131011</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="str">
         <f>B3</f>
-        <v>APXCAS2131001</v>
+        <v>APXCAS2131011</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="64.5" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="str">
         <f>B3</f>
-        <v>APXCAS2131001</v>
+        <v>APXCAS2131011</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="str">
         <f>D3</f>
-        <v>APXCAS2131001</v>
+        <v>APXCAS2131011</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
@@ -958,18 +958,18 @@
     <row r="6" spans="2:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="str">
         <f>"Cell# "&amp;Input!B7</f>
-        <v>Cell# 3</v>
+        <v>Cell# 1</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="10" t="str">
         <f>B6</f>
-        <v>Cell# 3</v>
+        <v>Cell# 1</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="/tKd7zyIL2ikjeKPWozriFnIzSvvJRvZ8zSC+evLMOxXsJPBwqK8m7ebOWYhouuqtA1S/Wt7yVcX/GXPYdZlWw==" saltValue="Phyqz+GiFI78OJtDEZclJw==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>

<commit_message>
Added auto SAP download
</commit_message>
<xml_diff>
--- a/templates/InstrumentSign_New.xlsx
+++ b/templates/InstrumentSign_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlam\OneDrive - Illumina, Inc\Documents\Github\Integration-1-Prep-Project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B85E75-BF82-4D00-A7FC-6A2296F921D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC65D96-995A-4757-B144-7B5C043B28C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t>CA 1.0</t>
   </si>
   <si>
-    <t>A01603</t>
-  </si>
-  <si>
-    <t>APXCAS2131011</t>
+    <t>A01605</t>
+  </si>
+  <si>
+    <t>APXCAS2134002</t>
   </si>
 </sst>
 </file>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>20578803</v>
+        <v>20578805</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -848,7 +848,7 @@
       </c>
       <c r="B7" s="21">
         <f>IF(MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3)=0,3,MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -903,45 +903,45 @@
     <row r="1" spans="2:4" ht="38.5" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="str">
         <f xml:space="preserve"> "PRO:"&amp;Input!B3</f>
-        <v>PRO:20578803</v>
+        <v>PRO:20578805</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="str">
         <f>B1</f>
-        <v>PRO:20578803</v>
+        <v>PRO:20578805</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="90.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="str">
         <f>Input!B4</f>
-        <v>A01603</v>
+        <v>A01605</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>A01603</v>
+        <v>A01605</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="str">
         <f>Input!B5</f>
-        <v>APXCAS2131011</v>
+        <v>APXCAS2134002</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="str">
         <f>B3</f>
-        <v>APXCAS2131011</v>
+        <v>APXCAS2134002</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="64.5" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="str">
         <f>B3</f>
-        <v>APXCAS2131011</v>
+        <v>APXCAS2134002</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="str">
         <f>D3</f>
-        <v>APXCAS2131011</v>
+        <v>APXCAS2134002</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
@@ -958,12 +958,12 @@
     <row r="6" spans="2:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="str">
         <f>"Cell# "&amp;Input!B7</f>
-        <v>Cell# 1</v>
+        <v>Cell# 3</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="10" t="str">
         <f>B6</f>
-        <v>Cell# 1</v>
+        <v>Cell# 3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added bat file to open SAP
</commit_message>
<xml_diff>
--- a/templates/InstrumentSign_New.xlsx
+++ b/templates/InstrumentSign_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlam\OneDrive - Illumina, Inc\Documents\Github\Integration-1-Prep-Project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC65D96-995A-4757-B144-7B5C043B28C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC602B2-D20E-4501-9BE5-D827CB40D282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Instrument SN:</t>
   </si>
@@ -66,10 +66,7 @@
     <t>CA 1.0</t>
   </si>
   <si>
-    <t>A01605</t>
-  </si>
-  <si>
-    <t>APXCAS2134002</t>
+    <t>A01606</t>
   </si>
 </sst>
 </file>
@@ -789,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>20578805</v>
+        <v>20581576</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -818,9 +815,7 @@
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="B5" s="15"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -848,7 +843,7 @@
       </c>
       <c r="B7" s="21">
         <f>IF(MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3)=0,3,MOD(_xlfn.NUMBERVALUE(RIGHT(B4,4)),3))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -903,45 +898,45 @@
     <row r="1" spans="2:4" ht="38.5" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="str">
         <f xml:space="preserve"> "PRO:"&amp;Input!B3</f>
-        <v>PRO:20578805</v>
+        <v>PRO:20581576</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="str">
         <f>B1</f>
-        <v>PRO:20578805</v>
+        <v>PRO:20581576</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="90.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="str">
         <f>Input!B4</f>
-        <v>A01605</v>
+        <v>A01606</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>A01605</v>
+        <v>A01606</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="5" t="str">
+      <c r="B3" s="5">
         <f>Input!B5</f>
-        <v>APXCAS2134002</v>
+        <v>0</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="5" t="str">
+      <c r="D3" s="5">
         <f>B3</f>
-        <v>APXCAS2134002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="str">
+      <c r="B4" s="6">
         <f>B3</f>
-        <v>APXCAS2134002</v>
+        <v>0</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6" t="str">
+      <c r="D4" s="6">
         <f>D3</f>
-        <v>APXCAS2134002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">
@@ -958,12 +953,12 @@
     <row r="6" spans="2:4" ht="43.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="10" t="str">
         <f>"Cell# "&amp;Input!B7</f>
-        <v>Cell# 3</v>
+        <v>Cell# 1</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="10" t="str">
         <f>B6</f>
-        <v>Cell# 3</v>
+        <v>Cell# 1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed code flow + removed features
- Added code to print on both sides.
- Program now calls 'integration prep.vbs' from parent folder.
- Print window is not used anymore
- 'Generate' also prints now
- New work flow is 'Edit SAP script' -> drag vbs script to SAP -> 'Generate'
</commit_message>
<xml_diff>
--- a/templates/InstrumentSign_New.xlsx
+++ b/templates/InstrumentSign_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlam\OneDrive - Illumina, Inc\Documents\Github\Integration-1-Prep-Project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC602B2-D20E-4501-9BE5-D827CB40D282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ED336E-711F-4F97-A390-09A1BDD5DB94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Instrument SN:</t>
   </si>
@@ -66,7 +66,10 @@
     <t>CA 1.0</t>
   </si>
   <si>
-    <t>A01606</t>
+    <t>A01612</t>
+  </si>
+  <si>
+    <t>APXCAS2134009</t>
   </si>
 </sst>
 </file>
@@ -786,7 +789,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>20581576</v>
+        <v>20583536</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -815,7 +818,9 @@
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
+      <c r="B5" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
@@ -898,45 +903,45 @@
     <row r="1" spans="2:4" ht="38.5" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="str">
         <f xml:space="preserve"> "PRO:"&amp;Input!B3</f>
-        <v>PRO:20581576</v>
+        <v>PRO:20583536</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="str">
         <f>B1</f>
-        <v>PRO:20581576</v>
+        <v>PRO:20583536</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="90.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="str">
         <f>Input!B4</f>
-        <v>A01606</v>
+        <v>A01612</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>A01606</v>
+        <v>A01612</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="5">
+      <c r="B3" s="5" t="str">
         <f>Input!B5</f>
-        <v>0</v>
+        <v>APXCAS2134009</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="5">
+      <c r="D3" s="5" t="str">
         <f>B3</f>
-        <v>0</v>
+        <v>APXCAS2134009</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="6">
+      <c r="B4" s="6" t="str">
         <f>B3</f>
-        <v>0</v>
+        <v>APXCAS2134009</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6">
+      <c r="D4" s="6" t="str">
         <f>D3</f>
-        <v>0</v>
+        <v>APXCAS2134009</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed material number handling
</commit_message>
<xml_diff>
--- a/templates/InstrumentSign_New.xlsx
+++ b/templates/InstrumentSign_New.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlam\OneDrive - Illumina, Inc\Documents\Github\Integration-1-Prep-Project\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5A4E4B-1A1C-4DB9-8507-5A3C124B8C61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA7274D-7BEF-4D0D-ADD3-5A1CE9330422}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Instrument SN:</t>
   </si>
@@ -66,10 +66,7 @@
     <t>CA 1.0</t>
   </si>
   <si>
-    <t>A01612</t>
-  </si>
-  <si>
-    <t>APXCAS2134009</t>
+    <t>A01672</t>
   </si>
 </sst>
 </file>
@@ -751,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -789,7 +786,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>20583536</v>
+        <v>20595735</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -818,8 +815,8 @@
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15" t="s">
-        <v>11</v>
+      <c r="B5" s="15">
+        <v>12341</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
@@ -888,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
@@ -903,45 +900,45 @@
     <row r="1" spans="2:4" ht="38.5" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="str">
         <f xml:space="preserve"> "PRO:"&amp;Input!B3</f>
-        <v>PRO:20583536</v>
+        <v>PRO:20595735</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="9" t="str">
         <f>B1</f>
-        <v>PRO:20583536</v>
+        <v>PRO:20595735</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="90.5" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="str">
         <f>Input!B4</f>
-        <v>A01612</v>
+        <v>A01672</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="2" t="str">
         <f>B2</f>
-        <v>A01612</v>
+        <v>A01672</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="5" t="str">
+      <c r="B3" s="5">
         <f>Input!B5</f>
-        <v>APXCAS2134009</v>
+        <v>12341</v>
       </c>
       <c r="C3" s="5"/>
-      <c r="D3" s="5" t="str">
+      <c r="D3" s="5">
         <f>B3</f>
-        <v>APXCAS2134009</v>
+        <v>12341</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="64.5" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="str">
+      <c r="B4" s="6">
         <f>B3</f>
-        <v>APXCAS2134009</v>
+        <v>12341</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6" t="str">
+      <c r="D4" s="6">
         <f>D3</f>
-        <v>APXCAS2134009</v>
+        <v>12341</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="100" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>